<commit_message>
Integration Feedback from Ciro
</commit_message>
<xml_diff>
--- a/tests/STN02/Dataset/Alignment.xlsx
+++ b/tests/STN02/Dataset/Alignment.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20400"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://engisiscom.sharepoint.com/sites/Engisis/Documenti condivisi/IFC/Technical Service/Phase III/Documents/BC002-Stationing on alignment/Dataset/B_con broken chainage/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\bSI-RailwayRoom\IFC4.x-IF\tests\STN02\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="446" documentId="13_ncr:1_{5F217189-E28F-4251-B661-372D328F598A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F75B8FF-CAC6-46F3-8E33-64D0A5877BF5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAFF1F1-429C-46E2-90A2-8323CB8C5760}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="5" xr2:uid="{060565B8-D44B-4C24-897B-88EAD87C1488}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="33120" windowHeight="18120" tabRatio="748" xr2:uid="{060565B8-D44B-4C24-897B-88EAD87C1488}"/>
   </bookViews>
   <sheets>
-    <sheet name="Check Table_Total" sheetId="7" r:id="rId1"/>
-    <sheet name="Check Table_before BC" sheetId="2" r:id="rId2"/>
-    <sheet name="Check Table_after BC" sheetId="6" r:id="rId3"/>
-    <sheet name="Alignment Horizontal Segment" sheetId="1" r:id="rId4"/>
-    <sheet name="Alignment Vertical Segment" sheetId="3" r:id="rId5"/>
-    <sheet name="Alignment Cant Segment" sheetId="4" r:id="rId6"/>
+    <sheet name="Alignment Horizontal Segment" sheetId="1" r:id="rId1"/>
+    <sheet name="Alignment Vertical Segment" sheetId="3" r:id="rId2"/>
+    <sheet name="Alignment Cant Segment" sheetId="4" r:id="rId3"/>
+    <sheet name="Check Table_Total" sheetId="7" r:id="rId4"/>
+    <sheet name="Check Table_before BC" sheetId="2" r:id="rId5"/>
+    <sheet name="Check Table_after BC" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,10 +46,19 @@
   <commentList>
     <comment ref="D3" authorId="0" shapeId="0" xr:uid="{BB76D2DA-6F80-4E47-A1B4-91DD0D4279D2}">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color theme="1"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <scheme val="minor"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     i had found these values that really look like dist along.</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -1337,48 +1346,48 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1393,12 +1402,9 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="35">
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
-    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -1443,6 +1449,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0000"/>
@@ -1948,7 +1957,7 @@
     <tableColumn id="1" xr3:uid="{42F768EF-4F15-43F5-A48A-F5C7BAD840BF}" name="ID"/>
     <tableColumn id="2" xr3:uid="{56E09658-E18B-4D1B-A850-0523F1E4ED28}" name="PredefinedType"/>
     <tableColumn id="3" xr3:uid="{F7788EBD-29A4-4BF7-A4B8-409DD97D6895}" name="Start Dist Along"/>
-    <tableColumn id="4" xr3:uid="{21BF728F-EB44-46F1-8B0B-B2470B4F5D30}" name="Horizontal Length" dataDxfId="8" totalsRowDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{21BF728F-EB44-46F1-8B0B-B2470B4F5D30}" name="Horizontal Length" dataDxfId="8" totalsRowDxfId="7"/>
     <tableColumn id="5" xr3:uid="{6FDB16A5-8281-4D22-B46B-AFA66BFE2283}" name="Start Cant left"/>
     <tableColumn id="6" xr3:uid="{90143F68-6B71-4DF8-B97B-5A0BF5358C03}" name="End Cant left"/>
     <tableColumn id="7" xr3:uid="{F9CDB949-CCD4-40C3-A8F3-628CF50D7BAC}" name="Start Cant right"/>
@@ -1960,10 +1969,10 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{751CA375-0DD6-4151-AB0A-9690F7A55A36}" name="Table108" displayName="Table108" ref="O3:O10" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{751CA375-0DD6-4151-AB0A-9690F7A55A36}" name="Table108" displayName="Table108" ref="O3:O10" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="O3:O10" xr:uid="{751CA375-0DD6-4151-AB0A-9690F7A55A36}"/>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{68DE499A-D808-4D97-B914-948A0A6B4EFF}" name="Type of Alignment Cant Segment" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{68DE499A-D808-4D97-B914-948A0A6B4EFF}" name="Type of Alignment Cant Segment" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1973,20 +1982,20 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{A136AF5A-648B-4E31-A9AF-3E1E1731FF1A}" name="Table16" displayName="Table16" ref="C27:I43" totalsRowShown="0">
   <autoFilter ref="C27:I43" xr:uid="{A136AF5A-648B-4E31-A9AF-3E1E1731FF1A}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{EBC3653B-5F1C-49F5-BA20-D7D079A07F46}" name="START" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{EBC3653B-5F1C-49F5-BA20-D7D079A07F46}" name="START" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{51C57841-8580-4CC8-B790-D67C465ED2CF}" name="raggio"/>
-    <tableColumn id="3" xr3:uid="{D9F1A893-19C3-408F-A51A-22A350C1AF1C}" name="cant ITF" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{7A0C1506-53DB-46F6-8119-1A2C987FB811}" name="Start Cant left" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{D9F1A893-19C3-408F-A51A-22A350C1AF1C}" name="cant ITF" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{7A0C1506-53DB-46F6-8119-1A2C987FB811}" name="Start Cant left" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{98775815-7744-415F-9563-05602D5AAD4C}" name="End Cant left"/>
     <tableColumn id="6" xr3:uid="{0086C3B8-87D2-4311-BBD7-7EA5D1F47055}" name="Start Cant right"/>
-    <tableColumn id="7" xr3:uid="{8C42B482-EB00-4E14-A3A1-09F102531DD0}" name="End Cant right" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{8C42B482-EB00-4E14-A3A1-09F102531DD0}" name="End Cant right" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2274,7 +2283,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2289,636 +2298,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC0D786-771C-4A3D-9D6B-5E4BA4F8571F}">
-  <dimension ref="A1:D44"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="62.53515625" customWidth="1"/>
-    <col min="2" max="2" width="22.23046875" customWidth="1"/>
-    <col min="3" max="3" width="26.4609375" customWidth="1"/>
-    <col min="4" max="4" width="21.15234375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="str">
-        <f>'Check Table_before BC'!B1</f>
-        <v>-0+153.1000</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <f>'Check Table_before BC'!B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <f>'Check Table_before BC'!B3</f>
-        <v>452270.18829999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <f>'Check Table_before BC'!B4</f>
-        <v>4539403.9473999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2" t="str">
-        <f>'Check Table_before BC'!B5</f>
-        <v>-0+153.1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <f>'Check Table_before BC'!B6</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" s="1" t="str">
-        <f>'Check Table_after BC'!B1</f>
-        <v>5+350.0000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" s="1">
-        <f>'Check Table_after BC'!B2</f>
-        <v>1029.3721</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>123</v>
-      </c>
-      <c r="B9" s="70">
-        <f>'Check Table_after BC'!B3</f>
-        <v>453202.52409999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" s="70">
-        <f>'Check Table_after BC'!B4</f>
-        <v>4539831.9287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B11" s="70" t="str">
-        <f>'Check Table_after BC'!B5</f>
-        <v>5+350.0000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="70">
-        <f>'Check Table_after BC'!B6</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="70" t="str">
-        <f>'Check Table_after BC'!B7</f>
-        <v>5+779.2225</v>
-      </c>
-      <c r="C13" s="68"/>
-      <c r="D13" s="69"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="70">
-        <f>B8+(5779.2225-5350)</f>
-        <v>1458.5945999999999</v>
-      </c>
-      <c r="C14" s="68"/>
-      <c r="D14" s="69"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="70">
-        <f>'Check Table_after BC'!B9</f>
-        <v>453616.16460000002</v>
-      </c>
-      <c r="C15" s="68"/>
-      <c r="D15" s="69"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="70">
-        <f>'Check Table_after BC'!B10</f>
-        <v>4539926.1048999997</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="70" t="str">
-        <f>'Check Table_after BC'!B11</f>
-        <v>5+779.2225</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18" s="70">
-        <f>'Check Table_after BC'!B12</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="2">
-        <f>'Check Table_before BC'!B13+'Check Table_after BC'!B13</f>
-        <v>1458.5946000000001</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2">
-        <f>'Check Table_before BC'!B14+'Check Table_after BC'!B14</f>
-        <v>1458.6178</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="2">
-        <f>'Check Table_before BC'!B15+'Check Table_after BC'!B15</f>
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B34" s="1"/>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.4">
-      <c r="B44" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K3c3c3bInformazione pubblica - Public information</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCE6198-CF24-4F7E-A72F-40F41CA83135}">
-  <dimension ref="A1:B33"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="57.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.4609375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>452270.18829999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>4539403.9473999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2">
-        <v>1029.3721</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2">
-        <v>453202.52409999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2">
-        <v>4539831.9287</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2">
-        <v>1029.3721</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2">
-        <v>1029.3860999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2">
-        <v>-3</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B19" s="1"/>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B23" s="1"/>
-    </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.4">
-      <c r="B33" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K3c3c3bInformazione pubblica - Public information</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1BC310-0D1D-4B1F-A382-BC5AB56CFEAA}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="1" max="1" width="45.15234375" customWidth="1"/>
-    <col min="2" max="2" width="62.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.69140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1029.3721</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
-        <v>453202.52409999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
-        <v>4539831.9287</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="2">
-        <v>453616.16460000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2">
-        <v>4539926.1048999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" s="2">
-        <v>429.22250000000003</v>
-      </c>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="2">
-        <v>429.23169999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.4">
-      <c r="A18" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K3c3c3bInformazione pubblica - Public information</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7816471-3137-4D8B-A5E6-BFF40F6053D4}">
   <dimension ref="A1:T42"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.3046875" customWidth="1"/>
-    <col min="2" max="2" width="6.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.53515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.4609375" customWidth="1"/>
-    <col min="6" max="6" width="22.53515625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="22.53515625" customWidth="1"/>
-    <col min="8" max="8" width="23.4609375" customWidth="1"/>
-    <col min="9" max="9" width="23.53515625" customWidth="1"/>
-    <col min="10" max="10" width="18.69140625" customWidth="1"/>
+    <col min="1" max="1" width="28.33203125" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.44140625" customWidth="1"/>
+    <col min="6" max="6" width="22.5546875" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5546875" customWidth="1"/>
+    <col min="8" max="8" width="23.44140625" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
     <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="14" max="14" width="34.3046875" customWidth="1"/>
-    <col min="16" max="16" width="8.69140625" customWidth="1"/>
-    <col min="19" max="20" width="20.69140625" customWidth="1"/>
+    <col min="14" max="14" width="34.33203125" customWidth="1"/>
+    <col min="16" max="16" width="8.6640625" customWidth="1"/>
+    <col min="19" max="20" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:20" ht="72" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -2926,23 +2331,23 @@
       <c r="C1" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="101"/>
       <c r="F1" s="33" t="s">
         <v>19</v>
       </c>
       <c r="G1" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="89" t="s">
+      <c r="H1" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="89"/>
+      <c r="I1" s="101"/>
       <c r="J1" s="33" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="19.850000000000001" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:20" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -2971,12 +2376,12 @@
       <c r="J2" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="S2" s="90" t="s">
+      <c r="S2" s="88" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="91"/>
-    </row>
-    <row r="3" spans="1:20" ht="43.85" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="T2" s="89"/>
+    </row>
+    <row r="3" spans="1:20" ht="43.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
@@ -3014,12 +2419,12 @@
       <c r="P3" s="5"/>
       <c r="Q3" s="5"/>
       <c r="R3" s="5"/>
-      <c r="S3" s="92" t="s">
+      <c r="S3" s="90" t="s">
         <v>115</v>
       </c>
-      <c r="T3" s="93"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.4">
+      <c r="T3" s="91"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -3064,7 +2469,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -3103,7 +2508,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -3142,7 +2547,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -3181,7 +2586,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>5</v>
       </c>
@@ -3214,7 +2619,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -3247,7 +2652,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -3280,7 +2685,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -3313,8 +2718,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="97" t="s">
+    <row r="12" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="95" t="s">
         <v>128</v>
       </c>
       <c r="B12" s="15">
@@ -3349,8 +2754,8 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.4">
-      <c r="A13" s="98"/>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A13" s="96"/>
       <c r="B13">
         <v>10</v>
       </c>
@@ -3380,7 +2785,7 @@
         <v>50.512999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="47"/>
       <c r="B14">
         <v>11</v>
@@ -3411,7 +2816,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="47"/>
       <c r="B15">
         <v>12</v>
@@ -3442,7 +2847,7 @@
         <v>172.82239999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="47"/>
       <c r="B16">
         <v>13</v>
@@ -3473,7 +2878,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="47"/>
       <c r="B17">
         <v>14</v>
@@ -3504,13 +2909,13 @@
         <v>85.887100000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="17"/>
       <c r="J18" s="2"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="B19" s="85" t="s">
         <v>129</v>
       </c>
@@ -3526,36 +2931,36 @@
         <v>1458.5945999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D20" s="87"/>
       <c r="E20" s="87"/>
       <c r="F20" s="87"/>
       <c r="G20" s="87"/>
       <c r="H20" s="87"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D21" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="99" t="s">
+      <c r="E21" s="97" t="s">
         <v>61</v>
       </c>
-      <c r="F21" s="100"/>
-      <c r="G21" s="100"/>
-      <c r="H21" s="101"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="99"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D22" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="E22" s="94" t="s">
+      <c r="E22" s="92" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="95"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="96"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="F22" s="93"/>
+      <c r="G22" s="93"/>
+      <c r="H22" s="94"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D23" s="49" t="s">
         <v>62</v>
       </c>
@@ -3572,7 +2977,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D24" s="50" t="str">
         <f t="shared" ref="D24:D32" si="1">F4</f>
         <v>77.723137g</v>
@@ -3593,7 +2998,7 @@
         <v>0.34992414572913133</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D25" s="51" t="str">
         <f t="shared" si="1"/>
         <v>77.723137g</v>
@@ -3614,7 +3019,7 @@
         <v>0.34992414572913133</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D26" s="50" t="str">
         <f t="shared" si="1"/>
         <v>76.449897g</v>
@@ -3635,7 +3040,7 @@
         <v>0.36992415288041447</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D27" s="51" t="str">
         <f t="shared" si="1"/>
         <v>64.133567g</v>
@@ -3656,7 +3061,7 @@
         <v>0.56338861211635272</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D28" s="50" t="str">
         <f t="shared" si="1"/>
         <v>62.860327g</v>
@@ -3677,7 +3082,7 @@
         <v>0.58338861926763597</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D29" s="51" t="str">
         <f t="shared" si="1"/>
         <v>62.860327g</v>
@@ -3698,7 +3103,7 @@
         <v>0.58338861926763597</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D30" s="50" t="str">
         <f t="shared" si="1"/>
         <v>64.133567g</v>
@@ -3719,7 +3124,7 @@
         <v>0.56338861211635272</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="D31" s="51" t="str">
         <f t="shared" si="1"/>
         <v>71.100208g</v>
@@ -3740,8 +3145,8 @@
         <v>0.45395687118736539</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="C32" s="97" t="s">
+    <row r="32" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C32" s="95" t="s">
         <v>128</v>
       </c>
       <c r="D32" s="75" t="str">
@@ -3764,8 +3169,8 @@
         <v>0.43395686403608202</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="C33" s="98"/>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C33" s="96"/>
       <c r="D33" s="71" t="s">
         <v>47</v>
       </c>
@@ -3785,7 +3190,7 @@
         <v>0.43395686403608202</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D34" s="50" t="s">
         <v>47</v>
       </c>
@@ -3805,7 +3210,7 @@
         <v>0.43395686403608202</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D35" s="51" t="s">
         <v>118</v>
       </c>
@@ -3825,7 +3230,7 @@
         <v>0.38395686186583688</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D36" s="50" t="s">
         <v>119</v>
       </c>
@@ -3846,7 +3251,7 @@
       </c>
       <c r="I36" s="4"/>
     </row>
-    <row r="37" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D37" s="52" t="s">
         <v>120</v>
       </c>
@@ -3867,34 +3272,34 @@
       </c>
       <c r="I37" s="4"/>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.3">
       <c r="E38" s="57"/>
       <c r="F38" s="40"/>
       <c r="G38" s="40"/>
       <c r="H38" s="40"/>
     </row>
-    <row r="39" spans="3:9" ht="20.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="3:9" ht="21" x14ac:dyDescent="0.4">
       <c r="D39" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="D40" s="88" t="s">
+    <row r="40" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D40" s="100" t="s">
         <v>66</v>
       </c>
-      <c r="E40" s="88"/>
-      <c r="F40" s="88"/>
-      <c r="G40" s="88"/>
-      <c r="H40" s="88"/>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.4">
-      <c r="D41" s="88"/>
-      <c r="E41" s="88"/>
-      <c r="F41" s="88"/>
-      <c r="G41" s="88"/>
-      <c r="H41" s="88"/>
-    </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.4">
+      <c r="E40" s="100"/>
+      <c r="F40" s="100"/>
+      <c r="G40" s="100"/>
+      <c r="H40" s="100"/>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="D41" s="100"/>
+      <c r="E41" s="100"/>
+      <c r="F41" s="100"/>
+      <c r="G41" s="100"/>
+      <c r="H41" s="100"/>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.3">
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
       <c r="F42" s="12"/>
@@ -3903,15 +3308,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="E21:H21"/>
     <mergeCell ref="D40:H41"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="S2:T2"/>
     <mergeCell ref="S3:T3"/>
     <mergeCell ref="E22:H22"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="E21:H21"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <dataValidations disablePrompts="1" count="1">
@@ -3929,7 +3334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EA0FABE-707B-4498-A8EE-9913D50761AF}">
   <dimension ref="A1:I17"/>
   <sheetViews>
@@ -3937,20 +3342,20 @@
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.4609375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.69140625" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="24" customWidth="1"/>
-    <col min="6" max="6" width="17.53515625" customWidth="1"/>
+    <col min="6" max="6" width="17.5546875" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="18.765625" customWidth="1"/>
-    <col min="9" max="9" width="24.4609375" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" customWidth="1"/>
+    <col min="9" max="9" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -3965,7 +3370,7 @@
       <c r="H1" s="34"/>
       <c r="I1" s="34"/>
     </row>
-    <row r="2" spans="1:9" ht="72.900000000000006" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -3992,7 +3397,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="53.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="18" t="s">
         <v>30</v>
@@ -4019,7 +3424,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>50</v>
       </c>
@@ -4048,7 +3453,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>51</v>
       </c>
@@ -4077,7 +3482,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>50</v>
       </c>
@@ -4106,7 +3511,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>51</v>
       </c>
@@ -4135,8 +3540,8 @@
         <v>-5000</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="97" t="s">
+    <row r="8" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="95" t="s">
         <v>128</v>
       </c>
       <c r="B8" s="80">
@@ -4164,8 +3569,8 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A9" s="98"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="96"/>
       <c r="B9" s="76">
         <v>6</v>
       </c>
@@ -4192,7 +3597,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>51</v>
       </c>
@@ -4222,7 +3627,7 @@
         <v>-5000</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>50</v>
       </c>
@@ -4252,7 +3657,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -4282,7 +3687,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>50</v>
       </c>
@@ -4312,7 +3717,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="85" t="s">
         <v>129</v>
       </c>
@@ -4327,7 +3732,7 @@
       <c r="H15" s="85"/>
       <c r="I15" s="85"/>
     </row>
-    <row r="17" spans="5:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
       <c r="E17" s="2"/>
     </row>
   </sheetData>
@@ -4347,35 +3752,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A98A46F9-E4F4-4678-840A-79FD8A384A52}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView topLeftCell="B13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.23046875" customWidth="1"/>
-    <col min="4" max="4" width="18.53515625" customWidth="1"/>
-    <col min="5" max="5" width="21.3046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.3046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.4609375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.53515625" customWidth="1"/>
-    <col min="11" max="11" width="43.765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="33.3046875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.3046875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.4609375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.3046875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.21875" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.5546875" customWidth="1"/>
+    <col min="11" max="11" width="43.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="43.75" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:22" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>17</v>
       </c>
@@ -4384,15 +3789,15 @@
       </c>
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
-      <c r="F1" s="89" t="s">
+      <c r="F1" s="101" t="s">
         <v>82</v>
       </c>
-      <c r="G1" s="89"/>
-      <c r="H1" s="89"/>
-      <c r="I1" s="89"/>
+      <c r="G1" s="101"/>
+      <c r="H1" s="101"/>
+      <c r="I1" s="101"/>
       <c r="J1" s="34"/>
     </row>
-    <row r="2" spans="1:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:22" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>23</v>
       </c>
@@ -4405,17 +3810,17 @@
       <c r="E2" s="33" t="s">
         <v>85</v>
       </c>
-      <c r="F2" s="89" t="s">
+      <c r="F2" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="G2" s="89"/>
-      <c r="H2" s="89"/>
-      <c r="I2" s="89"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+      <c r="I2" s="101"/>
       <c r="J2" s="33" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="44.4" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:22" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
@@ -4466,7 +3871,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>1</v>
       </c>
@@ -4519,7 +3924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>2</v>
       </c>
@@ -4571,7 +3976,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>3</v>
       </c>
@@ -4621,7 +4026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>4</v>
       </c>
@@ -4673,7 +4078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>5</v>
       </c>
@@ -4725,7 +4130,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>6</v>
       </c>
@@ -4765,7 +4170,7 @@
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>7</v>
       </c>
@@ -4799,7 +4204,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>8</v>
       </c>
@@ -4830,8 +4235,8 @@
       </c>
       <c r="J11" s="17"/>
     </row>
-    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="97" t="s">
+    <row r="12" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="95" t="s">
         <v>128</v>
       </c>
       <c r="B12" s="15">
@@ -4864,8 +4269,8 @@
       </c>
       <c r="J12" s="67"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
-      <c r="A13" s="98"/>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A13" s="96"/>
       <c r="B13">
         <v>10</v>
       </c>
@@ -4897,7 +4302,7 @@
       </c>
       <c r="L13" s="84"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>11</v>
       </c>
@@ -4929,7 +4334,7 @@
       </c>
       <c r="L14" s="84"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>12</v>
       </c>
@@ -4961,7 +4366,7 @@
       </c>
       <c r="L15" s="84"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>13</v>
       </c>
@@ -4993,7 +4398,7 @@
       </c>
       <c r="L16" s="84"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>14</v>
       </c>
@@ -5025,10 +4430,10 @@
       </c>
       <c r="L17" s="84"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B19" s="85" t="s">
         <v>129</v>
       </c>
@@ -5044,14 +4449,14 @@
       <c r="I19" s="85"/>
       <c r="J19" s="85"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="L23" s="2"/>
     </row>
-    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C26" s="103" t="s">
         <v>60</v>
       </c>
@@ -5064,7 +4469,7 @@
       <c r="H26" s="104"/>
       <c r="I26" s="105"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C27" s="13" t="s">
         <v>96</v>
       </c>
@@ -5087,7 +4492,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C28" s="13" t="s">
         <v>96</v>
       </c>
@@ -5110,7 +4515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>99</v>
       </c>
@@ -5137,7 +4542,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>100</v>
       </c>
@@ -5165,7 +4570,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>102</v>
       </c>
@@ -5192,7 +4597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>104</v>
       </c>
@@ -5218,7 +4623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -5245,7 +4650,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -5273,7 +4678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>109</v>
       </c>
@@ -5300,7 +4705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C36" s="13" t="s">
         <v>107</v>
       </c>
@@ -5323,8 +4728,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A37" s="97" t="s">
+    <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="95" t="s">
         <v>128</v>
       </c>
       <c r="B37" s="102"/>
@@ -5350,8 +4755,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
-      <c r="A38" s="97"/>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="95"/>
       <c r="B38" s="102"/>
       <c r="C38" s="62" t="s">
         <v>96</v>
@@ -5375,7 +4780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C39" s="13" t="s">
         <v>101</v>
       </c>
@@ -5399,7 +4804,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C40" s="13" t="s">
         <v>103</v>
       </c>
@@ -5424,7 +4829,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C41" s="13" t="s">
         <v>105</v>
       </c>
@@ -5448,7 +4853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C42" s="13" t="s">
         <v>107</v>
       </c>
@@ -5471,7 +4876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C43" s="14" t="s">
         <v>110</v>
       </c>
@@ -5509,6 +4914,612 @@
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDC0D786-771C-4A3D-9D6B-5E4BA4F8571F}">
+  <dimension ref="A1:D44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="62.5546875" customWidth="1"/>
+    <col min="2" max="2" width="22.21875" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" customWidth="1"/>
+    <col min="4" max="4" width="21.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="str">
+        <f>'Check Table_before BC'!B1</f>
+        <v>-0+153.1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <f>'Check Table_before BC'!B2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <f>'Check Table_before BC'!B3</f>
+        <v>452270.18829999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <f>'Check Table_before BC'!B4</f>
+        <v>4539403.9473999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2" t="str">
+        <f>'Check Table_before BC'!B5</f>
+        <v>-0+153.1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <f>'Check Table_before BC'!B6</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f>'Check Table_after BC'!B1</f>
+        <v>5+350.0000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="1">
+        <f>'Check Table_after BC'!B2</f>
+        <v>1029.3721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="70">
+        <f>'Check Table_after BC'!B3</f>
+        <v>453202.52409999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="70">
+        <f>'Check Table_after BC'!B4</f>
+        <v>4539831.9287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="70" t="str">
+        <f>'Check Table_after BC'!B5</f>
+        <v>5+350.0000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="70">
+        <f>'Check Table_after BC'!B6</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="70" t="str">
+        <f>'Check Table_after BC'!B7</f>
+        <v>5+779.2225</v>
+      </c>
+      <c r="C13" s="68"/>
+      <c r="D13" s="69"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="70">
+        <f>B8+(5779.2225-5350)</f>
+        <v>1458.5945999999999</v>
+      </c>
+      <c r="C14" s="68"/>
+      <c r="D14" s="69"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="70">
+        <f>'Check Table_after BC'!B9</f>
+        <v>453616.16460000002</v>
+      </c>
+      <c r="C15" s="68"/>
+      <c r="D15" s="69"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="70">
+        <f>'Check Table_after BC'!B10</f>
+        <v>4539926.1048999997</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="70" t="str">
+        <f>'Check Table_after BC'!B11</f>
+        <v>5+779.2225</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="70">
+        <f>'Check Table_after BC'!B12</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="2">
+        <f>'Check Table_before BC'!B13+'Check Table_after BC'!B13</f>
+        <v>1458.5946000000001</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2">
+        <f>'Check Table_before BC'!B14+'Check Table_after BC'!B14</f>
+        <v>1458.6178</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2">
+        <f>'Check Table_before BC'!B15+'Check Table_after BC'!B15</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B30" s="1"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K3c3c3bInformazione pubblica - Public information</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DCE6198-CF24-4F7E-A72F-40F41CA83135}">
+  <dimension ref="A1:B33"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="57.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>452270.18829999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4539403.9473999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1029.3721</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>453202.52409999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4539831.9287</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>1029.3721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
+        <v>1029.3860999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="1"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B33" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K3c3c3bInformazione pubblica - Public information</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC1BC310-0D1D-4B1F-A382-BC5AB56CFEAA}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="45.109375" customWidth="1"/>
+    <col min="2" max="2" width="62.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1029.3721</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>453202.52409999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>4539831.9287</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="2">
+        <v>453616.16460000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4539926.1048999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2">
+        <v>429.22250000000003</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="2">
+        <v>429.23169999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K3c3c3bInformazione pubblica - Public information</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>